<commit_message>
Actualizaciones y corrección de errores
</commit_message>
<xml_diff>
--- a/servidor/plantillasVacias/Dispositivos.xlsx
+++ b/servidor/plantillasVacias/Dispositivos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jennytipan\Desktop\ProyectoFulltime\FullTimeV3\servidor\plantillasVacias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA31701-DDEF-4857-BAC5-5BF65507C9B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E9B05-2733-423B-8BE7-2A09908F65D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>nombre</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>modelo1 (opcional)</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>numero_acciones</t>
+  </si>
+  <si>
+    <t>(no ingresar nada)</t>
   </si>
 </sst>
 </file>
@@ -454,110 +463,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>8090</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="b">
+      <c r="L2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +600,7 @@
           <x14:formula1>
             <xm:f>Selectores!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1588</xm:sqref>
+          <xm:sqref>L2:L1588</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>